<commit_message>
Updated script on 21/11
</commit_message>
<xml_diff>
--- a/7rMartSuperMarket/src/main/resources/TestData.xlsx
+++ b/7rMartSuperMarket/src/main/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomcy\git\Selenium_Project\7rMartSuperMarket\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88B7B58-DD45-406A-86CC-E32BFE636E26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F6F161-05C7-40C8-8391-D22BD9D4F30D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D33EEA85-A74F-444B-8BDC-AA14F7F1605D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="4" xr2:uid="{D33EEA85-A74F-444B-8BDC-AA14F7F1605D}"/>
   </bookViews>
   <sheets>
     <sheet name="loginpage" sheetId="1" r:id="rId1"/>
@@ -110,7 +110,7 @@
     <t>Apple</t>
   </si>
   <si>
-    <t>rtrtrtr</t>
+    <t>nayana</t>
   </si>
 </sst>
 </file>
@@ -464,7 +464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2C6822D-6C1E-4E5E-A2A6-9B8F0BCCF016}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -634,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CCC7FBD-3161-4517-821E-B9882B708E83}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -653,7 +653,7 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>